<commit_message>
EPBDS-8247 Implement ability to store description of Conditions and Return and Input data separately from Rules table. Transponse Conditions/Returns table support added.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Return_2.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Return_2.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkamalov\.openl\user-workspace\DEFAULT\EPBDS-8247_Conditions_Return_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6973370-1F7D-45A2-A29B-24380A0E792E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106CF83F-C5DE-42FF-BB60-307F620A0068}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="945" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7410" yWindow="4365" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Conditions</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>SmartRules DoubleValue test1(Double p1, Integer p2)</t>
-  </si>
-  <si>
-    <t>Always TRUE</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>SmartRules DoubleValue test3(Double p1, Integer p2)</t>
@@ -96,7 +90,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -123,13 +116,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921" rgb="4F81BD"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,15 +215,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
     <border>
-      <bottom style="medium"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -253,6 +258,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,38 +306,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -307,67 +327,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="1" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -735,52 +719,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F354967-CCBB-4C8D-AC6A-190478DBA6AE}">
-  <dimension ref="C3:I51"/>
+  <dimension ref="C3:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="35.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="3:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="10" t="s">
@@ -797,7 +781,7 @@
       <c r="H6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="28"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C7" s="11" t="s">
@@ -810,7 +794,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="28"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
@@ -825,7 +809,7 @@
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="28"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
@@ -838,22 +822,22 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="29"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="16" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
@@ -862,7 +846,7 @@
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="19">
+      <c r="C19" s="24">
         <v>1</v>
       </c>
       <c r="D19" s="20"/>
@@ -874,7 +858,7 @@
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="19">
+      <c r="C20" s="24">
         <v>2</v>
       </c>
       <c r="D20" s="20"/>
@@ -886,7 +870,7 @@
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="19">
+      <c r="C21" s="24">
         <v>3</v>
       </c>
       <c r="D21" s="20"/>
@@ -898,7 +882,7 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="19">
+      <c r="C22" s="24">
         <v>4</v>
       </c>
       <c r="D22" s="20"/>
@@ -910,7 +894,7 @@
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="19">
+      <c r="C23" s="24">
         <v>5</v>
       </c>
       <c r="D23" s="20"/>
@@ -922,7 +906,7 @@
       </c>
     </row>
     <row r="24" spans="3:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="21">
+      <c r="C24" s="30">
         <v>6</v>
       </c>
       <c r="D24" s="22"/>
@@ -936,27 +920,27 @@
     <row r="26" spans="3:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="3:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C28" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
+      <c r="C28" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C29" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="18"/>
+      <c r="C29" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="29"/>
       <c r="E29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C30" s="19">
+      <c r="C30" s="24">
         <v>1</v>
       </c>
       <c r="D30" s="20"/>
@@ -968,7 +952,7 @@
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C31" s="19">
+      <c r="C31" s="24">
         <v>2</v>
       </c>
       <c r="D31" s="20"/>
@@ -980,7 +964,7 @@
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="19">
+      <c r="C32" s="24">
         <v>3</v>
       </c>
       <c r="D32" s="20"/>
@@ -992,7 +976,7 @@
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C33" s="19">
+      <c r="C33" s="24">
         <v>4</v>
       </c>
       <c r="D33" s="20"/>
@@ -1004,7 +988,7 @@
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C34" s="19">
+      <c r="C34" s="24">
         <v>5</v>
       </c>
       <c r="D34" s="20"/>
@@ -1016,7 +1000,7 @@
       </c>
     </row>
     <row r="35" spans="3:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="21">
+      <c r="C35" s="30">
         <v>6</v>
       </c>
       <c r="D35" s="22"/>
@@ -1030,6 +1014,23 @@
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -1040,23 +1041,6 @@
     <mergeCell ref="H6:I9"/>
     <mergeCell ref="F8:G9"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1064,17 +1048,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63C529D-8F6D-4385-8ECE-0B2A69A63EA5}">
-  <dimension ref="B3:H55"/>
+  <dimension ref="B3:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="50.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1089,136 +1073,143 @@
       <c r="G4" s="9"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32" t="s">
+      <c r="E6" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="30" t="s">
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="E8" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-    </row>
-    <row r="15" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-    </row>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="16" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" t="n" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="E18" t="n" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="21" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C19" s="52"/>
-      <c r="D19" t="n" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="50"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="47"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C22" s="43"/>
-    </row>
-    <row r="23" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="22"/>
-    </row>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B19" s="24">
+        <v>1</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="42">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12">
+        <v>2</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="G5:H8"/>
-    <mergeCell ref="B17:C17"/>
+  <mergeCells count="13">
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H9"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="B17:E17"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>